<commit_message>
Commented out exam scheduling code and modified README.md
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_DSAI_timetable.xlsx
+++ b/backend/output_timetables/sem1_DSAI_timetable.xlsx
@@ -1422,7 +1422,7 @@
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="F6" s="8" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="F7" s="9" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L106]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -2454,7 +2454,7 @@
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L106]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -3435,7 +3435,7 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L106]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="C6" s="12" t="inlineStr">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L106]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">

</xml_diff>